<commit_message>
add nptg add overwrite option
</commit_message>
<xml_diff>
--- a/request spreadsheets/METrequest.xlsx
+++ b/request spreadsheets/METrequest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dft/Documents/Naptan stop templates and script/request spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dft/PycharmProjects/NaPTAN-xlsx-xml-import/request spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F60557-F75C-4846-95A4-2E23C8C09AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087D319E-9B7D-824C-8998-11E42CAAC130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="580" windowWidth="33600" windowHeight="19200" xr2:uid="{33265FF0-805D-DC45-B245-6395E91CA3D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>CommonName</t>
   </si>
@@ -113,16 +113,10 @@
     <t>Barking Testside new</t>
   </si>
   <si>
-    <t>Street</t>
-  </si>
-  <si>
     <t>Longitude</t>
   </si>
   <si>
     <t>Latitude</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>9400ZZBPCLP1</t>
@@ -500,15 +494,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29084EE-9877-FD4C-B31E-5145E7B44BBE}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -522,51 +516,48 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
@@ -575,63 +566,60 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="G2" s="2">
+        <v>546944</v>
+      </c>
       <c r="H2" s="2">
-        <v>546944</v>
+        <v>182222</v>
       </c>
       <c r="I2" s="2">
-        <v>182222</v>
+        <v>-2.4419676053099999</v>
       </c>
       <c r="J2" s="2">
-        <v>-2.4419676053099999</v>
+        <v>54.814594497770003</v>
       </c>
       <c r="K2" s="2">
-        <v>54.814594497770003</v>
-      </c>
-      <c r="L2" s="2">
         <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <v>44652</v>
       </c>
       <c r="M2" s="3">
         <v>44652</v>
       </c>
-      <c r="N2" s="3">
-        <v>44652</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="2">
+      <c r="O2" s="2">
         <v>0</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R2">
+      <c r="Q2">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{83DC678A-362C-6D49-A1CC-182F3C0C4F23}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{83DC678A-362C-6D49-A1CC-182F3C0C4F23}">
       <formula1>"1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{9247FB47-D695-0840-836B-8FF0E67DC642}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576" xr:uid="{9247FB47-D695-0840-836B-8FF0E67DC642}">
       <formula1>"new, revise"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q1048576" xr:uid="{7D82AD20-8742-E041-976A-38E047E192B5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576" xr:uid="{7D82AD20-8742-E041-976A-38E047E192B5}">
       <formula1>"active, inactive"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{0B63B883-5D44-1240-8E0A-00A1B1E2BAC6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{0B63B883-5D44-1240-8E0A-00A1B1E2BAC6}">
       <formula1>"MET"</formula1>
     </dataValidation>
   </dataValidations>
@@ -672,10 +660,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -695,7 +683,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>

</xml_diff>